<commit_message>
finished translations of sentences in Tisu Diary and SIL booklets
</commit_message>
<xml_diff>
--- a/exports/L099-tok-result-csv.xlsx
+++ b/exports/L099-tok-result-csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackbowers/Box Sync/Language_Data/Mixtepec_Mixtec/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC00E80F-7986-DD4D-9675-83923B6FCCB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47459366-C499-4A40-9EEB-860272C4C0AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{B4304F77-315D-D840-818C-F12373B6B0BD}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{B4304F77-315D-D840-818C-F12373B6B0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="331">
   <si>
     <t>Orth</t>
   </si>
@@ -1042,6 +1042,9 @@
   </si>
   <si>
     <t>ñasi'i</t>
+  </si>
+  <si>
+    <t>add sentence to TEI after glossed</t>
   </si>
 </sst>
 </file>
@@ -1158,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1196,6 +1199,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1516,26 +1582,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D50492-77BB-1741-BB87-DA44A2A761EA}">
   <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="97" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="97" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="21" customWidth="1"/>
     <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="75.6640625" style="31" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="78.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1612,7 @@
       <c r="C1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>321</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1572,7 +1639,7 @@
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="30" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1592,7 +1659,7 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="31" t="s">
         <v>15</v>
       </c>
       <c r="N2" t="s">
@@ -1612,7 +1679,7 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="31" t="s">
         <v>19</v>
       </c>
       <c r="N3" t="s">
@@ -1629,7 +1696,7 @@
       <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="31" t="s">
         <v>25</v>
       </c>
       <c r="N4" t="s">
@@ -1645,7 +1712,7 @@
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="D5" s="22"/>
       <c r="E5" s="14" t="s">
         <v>85</v>
       </c>
@@ -1658,7 +1725,7 @@
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="32" t="s">
         <v>42</v>
       </c>
       <c r="N5" s="14" t="s">
@@ -1674,7 +1741,7 @@
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="14" t="s">
         <v>88</v>
       </c>
@@ -1687,7 +1754,7 @@
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="32" t="s">
         <v>60</v>
       </c>
       <c r="N6" s="14" t="s">
@@ -1707,7 +1774,7 @@
       <c r="H7" t="s">
         <v>36</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="31" t="s">
         <v>37</v>
       </c>
       <c r="N7" t="s">
@@ -1727,7 +1794,7 @@
       <c r="H8" t="s">
         <v>36</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="31" t="s">
         <v>31</v>
       </c>
       <c r="N8" t="s">
@@ -1750,7 +1817,7 @@
       <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="31" t="s">
         <v>31</v>
       </c>
       <c r="N9" t="s">
@@ -1773,7 +1840,7 @@
       <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="31" t="s">
         <v>31</v>
       </c>
       <c r="N10" t="s">
@@ -1793,7 +1860,7 @@
       <c r="H11" t="s">
         <v>92</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N11" t="s">
@@ -1813,7 +1880,7 @@
       <c r="H12" t="s">
         <v>92</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N12" t="s">
@@ -1829,7 +1896,7 @@
       </c>
       <c r="B13"/>
       <c r="C13"/>
-      <c r="D13"/>
+      <c r="D13" s="21"/>
       <c r="E13" t="s">
         <v>100</v>
       </c>
@@ -1842,7 +1909,7 @@
       <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
-      <c r="M13" t="s">
+      <c r="M13" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N13" t="s">
@@ -1862,7 +1929,7 @@
       <c r="H14" t="s">
         <v>101</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N14" t="s">
@@ -1878,7 +1945,7 @@
       </c>
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15"/>
+      <c r="D15" s="21"/>
       <c r="E15" t="s">
         <v>100</v>
       </c>
@@ -1895,7 +1962,7 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="L15"/>
-      <c r="M15" t="s">
+      <c r="M15" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N15" t="s">
@@ -1911,7 +1978,7 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="8" t="s">
         <v>103</v>
       </c>
@@ -1924,7 +1991,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="33" t="s">
         <v>60</v>
       </c>
       <c r="N16" s="8" t="s">
@@ -1944,7 +2011,7 @@
       <c r="H17" t="s">
         <v>95</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N17" t="s">
@@ -1964,7 +2031,7 @@
       <c r="H18" t="s">
         <v>95</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N18" t="s">
@@ -1984,7 +2051,7 @@
       <c r="H19" t="s">
         <v>95</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N19" t="s">
@@ -2004,7 +2071,7 @@
       <c r="H20" t="s">
         <v>113</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="31" t="s">
         <v>37</v>
       </c>
       <c r="N20" t="s">
@@ -2024,7 +2091,7 @@
       <c r="H21" t="s">
         <v>116</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="31" t="s">
         <v>70</v>
       </c>
       <c r="N21" t="s">
@@ -2040,7 +2107,7 @@
       </c>
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22"/>
+      <c r="D22" s="21"/>
       <c r="E22" t="s">
         <v>120</v>
       </c>
@@ -2061,7 +2128,7 @@
       </c>
       <c r="K22"/>
       <c r="L22"/>
-      <c r="M22" t="s">
+      <c r="M22" s="31" t="s">
         <v>77</v>
       </c>
       <c r="N22" t="s">
@@ -2075,13 +2142,14 @@
       <c r="A23" s="13" t="s">
         <v>124</v>
       </c>
+      <c r="D23" s="22"/>
       <c r="E23" s="14" t="s">
         <v>125</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="32" t="s">
         <v>42</v>
       </c>
       <c r="N23" s="14" t="s">
@@ -2097,7 +2165,7 @@
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="16" t="s">
         <v>128</v>
       </c>
@@ -2110,7 +2178,7 @@
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
-      <c r="M24" s="16" t="s">
+      <c r="M24" s="34" t="s">
         <v>31</v>
       </c>
       <c r="N24" s="16" t="s">
@@ -2136,7 +2204,7 @@
       <c r="I25" t="s">
         <v>98</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N25" t="s">
@@ -2157,7 +2225,7 @@
       <c r="H26" t="s">
         <v>98</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N26" t="s">
@@ -2177,7 +2245,7 @@
       <c r="H27" t="s">
         <v>98</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N27" t="s">
@@ -2197,7 +2265,7 @@
       <c r="H28" t="s">
         <v>98</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N28" t="s">
@@ -2217,7 +2285,7 @@
       <c r="H29" t="s">
         <v>41</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N29" t="s">
@@ -2237,7 +2305,7 @@
       <c r="H30" t="s">
         <v>41</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="31" t="s">
         <v>21</v>
       </c>
       <c r="N30" t="s">
@@ -2257,7 +2325,7 @@
       <c r="H31" t="s">
         <v>41</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="31" t="s">
         <v>22</v>
       </c>
       <c r="N31" t="s">
@@ -2271,6 +2339,7 @@
       <c r="A32" s="13" t="s">
         <v>141</v>
       </c>
+      <c r="D32" s="22"/>
       <c r="E32" s="14" t="s">
         <v>142</v>
       </c>
@@ -2283,7 +2352,7 @@
       <c r="I32" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="M32" s="14" t="s">
+      <c r="M32" s="32" t="s">
         <v>42</v>
       </c>
       <c r="N32" s="14" t="s">
@@ -2297,13 +2366,14 @@
       <c r="A33" s="13" t="s">
         <v>144</v>
       </c>
+      <c r="D33" s="22"/>
       <c r="E33" s="14" t="s">
         <v>145</v>
       </c>
       <c r="H33" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="32" t="s">
         <v>37</v>
       </c>
       <c r="N33" s="14" t="s">
@@ -2319,7 +2389,7 @@
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="4" t="s">
         <v>148</v>
       </c>
@@ -2332,7 +2402,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="35" t="s">
         <v>73</v>
       </c>
       <c r="N34" s="4" t="s">
@@ -2352,7 +2422,7 @@
       <c r="H35" t="s">
         <v>149</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M35" s="31" t="s">
         <v>73</v>
       </c>
       <c r="N35" t="s">
@@ -2368,7 +2438,7 @@
       </c>
       <c r="B36"/>
       <c r="C36"/>
-      <c r="D36"/>
+      <c r="D36" s="21"/>
       <c r="E36" t="s">
         <v>148</v>
       </c>
@@ -2381,7 +2451,7 @@
       <c r="J36"/>
       <c r="K36"/>
       <c r="L36"/>
-      <c r="M36" t="s">
+      <c r="M36" s="31" t="s">
         <v>77</v>
       </c>
       <c r="N36" t="s">
@@ -2395,13 +2465,14 @@
       <c r="A37" s="13" t="s">
         <v>150</v>
       </c>
+      <c r="D37" s="22"/>
       <c r="E37" s="14" t="s">
         <v>151</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="M37" s="14" t="s">
+      <c r="M37" s="32" t="s">
         <v>153</v>
       </c>
       <c r="N37" s="14" t="s">
@@ -2427,7 +2498,7 @@
       <c r="I38" t="s">
         <v>254</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="31" t="s">
         <v>153</v>
       </c>
       <c r="N38" t="s">
@@ -2459,7 +2530,7 @@
       <c r="J39" t="s">
         <v>119</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M39" s="31" t="s">
         <v>77</v>
       </c>
       <c r="N39" t="s">
@@ -2485,7 +2556,7 @@
       <c r="I40" t="s">
         <v>289</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M40" s="31" t="s">
         <v>77</v>
       </c>
       <c r="N40" t="s">
@@ -2501,7 +2572,7 @@
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="4" t="s">
         <v>118</v>
       </c>
@@ -2518,7 +2589,7 @@
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="35" t="s">
         <v>73</v>
       </c>
       <c r="N41" s="4" t="s">
@@ -2544,7 +2615,7 @@
       <c r="I42" t="s">
         <v>123</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M42" s="31" t="s">
         <v>73</v>
       </c>
       <c r="N42" t="s">
@@ -2570,7 +2641,7 @@
       <c r="I43" t="s">
         <v>123</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M43" s="31" t="s">
         <v>73</v>
       </c>
       <c r="N43" t="s">
@@ -2602,7 +2673,7 @@
       <c r="J44" t="s">
         <v>171</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" s="31" t="s">
         <v>70</v>
       </c>
       <c r="N44" t="s">
@@ -2616,6 +2687,7 @@
       <c r="A45" s="11" t="s">
         <v>311</v>
       </c>
+      <c r="D45" s="26"/>
       <c r="E45" s="12" t="s">
         <v>168</v>
       </c>
@@ -2625,7 +2697,7 @@
       <c r="H45" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="M45" s="12" t="s">
+      <c r="M45" s="36" t="s">
         <v>70</v>
       </c>
       <c r="N45" s="12" t="s">
@@ -2639,6 +2711,7 @@
       <c r="A46" s="11" t="s">
         <v>172</v>
       </c>
+      <c r="D46" s="26"/>
       <c r="E46" s="12" t="s">
         <v>173</v>
       </c>
@@ -2654,7 +2727,7 @@
       <c r="I46" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="M46" s="12" t="s">
+      <c r="M46" s="36" t="s">
         <v>70</v>
       </c>
       <c r="N46" s="12" t="s">
@@ -2670,7 +2743,7 @@
       </c>
       <c r="B47"/>
       <c r="C47"/>
-      <c r="D47"/>
+      <c r="D47" s="21"/>
       <c r="E47" t="s">
         <v>253</v>
       </c>
@@ -2687,7 +2760,7 @@
       <c r="J47"/>
       <c r="K47"/>
       <c r="L47"/>
-      <c r="M47" t="s">
+      <c r="M47" s="31" t="s">
         <v>153</v>
       </c>
       <c r="N47" t="s">
@@ -2707,7 +2780,7 @@
       <c r="H48" t="s">
         <v>305</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M48" s="31" t="s">
         <v>153</v>
       </c>
       <c r="N48" t="s">
@@ -2723,7 +2796,7 @@
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="D49" s="25"/>
       <c r="E49" s="4" t="s">
         <v>306</v>
       </c>
@@ -2736,7 +2809,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4" t="s">
+      <c r="M49" s="35" t="s">
         <v>47</v>
       </c>
       <c r="N49" s="4" t="s">
@@ -2752,7 +2825,7 @@
       </c>
       <c r="B50"/>
       <c r="C50"/>
-      <c r="D50"/>
+      <c r="D50" s="21"/>
       <c r="E50" t="s">
         <v>306</v>
       </c>
@@ -2765,7 +2838,7 @@
       <c r="J50"/>
       <c r="K50"/>
       <c r="L50"/>
-      <c r="M50" t="s">
+      <c r="M50" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N50" t="s">
@@ -2785,7 +2858,7 @@
       <c r="H51" t="s">
         <v>310</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M51" s="31" t="s">
         <v>31</v>
       </c>
       <c r="N51" t="s">
@@ -2799,13 +2872,14 @@
       <c r="A52" s="13" t="s">
         <v>317</v>
       </c>
+      <c r="D52" s="22"/>
       <c r="E52" s="14" t="s">
         <v>318</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="M52" s="14" t="s">
+      <c r="M52" s="32" t="s">
         <v>19</v>
       </c>
       <c r="N52" s="14" t="s">
@@ -2816,13 +2890,14 @@
       <c r="A53" s="13" t="s">
         <v>176</v>
       </c>
+      <c r="D53" s="22"/>
       <c r="E53" s="14" t="s">
         <v>177</v>
       </c>
       <c r="H53" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="M53" s="14" t="s">
+      <c r="M53" s="32" t="s">
         <v>47</v>
       </c>
       <c r="N53" s="14" t="s">
@@ -2842,7 +2917,7 @@
       <c r="H54" t="s">
         <v>314</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M54" s="31" t="s">
         <v>197</v>
       </c>
       <c r="N54" t="s">
@@ -2868,7 +2943,7 @@
       <c r="I55" t="s">
         <v>158</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M55" s="31" t="s">
         <v>159</v>
       </c>
       <c r="N55" t="s">
@@ -2888,7 +2963,7 @@
       <c r="H56" t="s">
         <v>158</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="31" t="s">
         <v>159</v>
       </c>
       <c r="N56" t="s">
@@ -2908,7 +2983,7 @@
       <c r="H57" t="s">
         <v>164</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M57" s="31" t="s">
         <v>47</v>
       </c>
       <c r="N57" t="s">
@@ -2924,7 +2999,7 @@
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="D58" s="25"/>
       <c r="E58" s="4" t="s">
         <v>163</v>
       </c>
@@ -2943,7 +3018,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-      <c r="M58" s="4" t="s">
+      <c r="M58" s="35" t="s">
         <v>47</v>
       </c>
       <c r="N58" s="4" t="s">
@@ -2963,7 +3038,7 @@
       <c r="H59" t="s">
         <v>164</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M59" s="31" t="s">
         <v>47</v>
       </c>
       <c r="N59" t="s">
@@ -2973,44 +3048,47 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:15" s="9" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="4" t="s">
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E60" s="10" t="s">
         <v>180</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
-      <c r="H60" s="4" t="s">
+      <c r="H60" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4" t="s">
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="N60" s="4" t="s">
+      <c r="N60" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O60" s="4"/>
+      <c r="O60" s="10"/>
     </row>
     <row r="61" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>181</v>
       </c>
+      <c r="D61" s="22"/>
       <c r="E61" s="14" t="s">
         <v>182</v>
       </c>
       <c r="H61" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="M61" s="14" t="s">
+      <c r="M61" s="32" t="s">
         <v>31</v>
       </c>
       <c r="N61" s="14" t="s">
@@ -3024,13 +3102,14 @@
       <c r="A62" s="13" t="s">
         <v>184</v>
       </c>
+      <c r="D62" s="22"/>
       <c r="E62" s="14" t="s">
         <v>185</v>
       </c>
       <c r="H62" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="M62" s="14" t="s">
+      <c r="M62" s="32" t="s">
         <v>25</v>
       </c>
       <c r="N62" s="14" t="s">
@@ -3050,7 +3129,7 @@
       <c r="H63" t="s">
         <v>186</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M63" s="31" t="s">
         <v>25</v>
       </c>
       <c r="N63" t="s">
@@ -3070,7 +3149,7 @@
       <c r="H64" t="s">
         <v>192</v>
       </c>
-      <c r="M64" t="s">
+      <c r="M64" s="31" t="s">
         <v>19</v>
       </c>
       <c r="N64" t="s">
@@ -3081,10 +3160,11 @@
       <c r="A65" s="13" t="s">
         <v>193</v>
       </c>
+      <c r="D65" s="22"/>
       <c r="E65" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="M65" s="14" t="s">
+      <c r="M65" s="32" t="s">
         <v>37</v>
       </c>
       <c r="N65" s="14" t="s">
@@ -3098,13 +3178,14 @@
       <c r="A66" s="17" t="s">
         <v>195</v>
       </c>
+      <c r="D66" s="28"/>
       <c r="E66" s="18" t="s">
         <v>196</v>
       </c>
       <c r="H66" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="M66" s="18" t="s">
+      <c r="M66" s="38" t="s">
         <v>197</v>
       </c>
       <c r="N66" s="18" t="s">
@@ -3118,13 +3199,14 @@
       <c r="A67" s="13" t="s">
         <v>208</v>
       </c>
+      <c r="D67" s="22"/>
       <c r="E67" s="14" t="s">
         <v>209</v>
       </c>
       <c r="H67" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="M67" s="14" t="s">
+      <c r="M67" s="32" t="s">
         <v>81</v>
       </c>
       <c r="N67" s="14" t="s">
@@ -3138,13 +3220,14 @@
       <c r="A68" s="13" t="s">
         <v>206</v>
       </c>
+      <c r="D68" s="22"/>
       <c r="E68" s="14" t="s">
         <v>202</v>
       </c>
       <c r="H68" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="M68" s="14" t="s">
+      <c r="M68" s="32" t="s">
         <v>65</v>
       </c>
       <c r="N68" s="14" t="s">
@@ -3176,7 +3259,7 @@
       <c r="J69" t="s">
         <v>205</v>
       </c>
-      <c r="M69" t="s">
+      <c r="M69" s="31" t="s">
         <v>135</v>
       </c>
       <c r="N69" t="s">
@@ -3208,7 +3291,7 @@
       <c r="J70" t="s">
         <v>245</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M70" s="31" t="s">
         <v>135</v>
       </c>
       <c r="N70" t="s">
@@ -3240,7 +3323,7 @@
       <c r="J71" t="s">
         <v>278</v>
       </c>
-      <c r="M71" t="s">
+      <c r="M71" s="31" t="s">
         <v>135</v>
       </c>
       <c r="N71" t="s">
@@ -3254,13 +3337,14 @@
       <c r="A72" s="13" t="s">
         <v>211</v>
       </c>
+      <c r="D72" s="22"/>
       <c r="E72" s="14" t="s">
         <v>212</v>
       </c>
       <c r="H72" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="M72" s="14" t="s">
+      <c r="M72" s="32" t="s">
         <v>65</v>
       </c>
       <c r="N72" s="14" t="s">
@@ -3274,6 +3358,7 @@
       <c r="A73" s="13" t="s">
         <v>214</v>
       </c>
+      <c r="D73" s="22"/>
       <c r="E73" s="14" t="s">
         <v>215</v>
       </c>
@@ -3283,7 +3368,7 @@
       <c r="I73" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="M73" s="14" t="s">
+      <c r="M73" s="32" t="s">
         <v>52</v>
       </c>
       <c r="N73" s="14" t="s">
@@ -3303,7 +3388,7 @@
       <c r="H74" t="s">
         <v>224</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M74" s="31" t="s">
         <v>56</v>
       </c>
       <c r="N74" t="s">
@@ -3329,7 +3414,7 @@
       <c r="H75" t="s">
         <v>222</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M75" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N75" t="s">
@@ -3355,7 +3440,7 @@
       <c r="H76" t="s">
         <v>222</v>
       </c>
-      <c r="M76" t="s">
+      <c r="M76" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N76" t="s">
@@ -3369,13 +3454,14 @@
       <c r="A77" s="13" t="s">
         <v>225</v>
       </c>
+      <c r="D77" s="22"/>
       <c r="E77" s="14" t="s">
         <v>226</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="M77" s="14" t="s">
+      <c r="M77" s="32" t="s">
         <v>197</v>
       </c>
       <c r="N77" s="14" t="s">
@@ -3395,7 +3481,7 @@
       <c r="H78" t="s">
         <v>230</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M78" s="31" t="s">
         <v>56</v>
       </c>
       <c r="N78" t="s">
@@ -3409,6 +3495,7 @@
       <c r="A79" s="13" t="s">
         <v>328</v>
       </c>
+      <c r="D79" s="22"/>
       <c r="E79" s="14" t="s">
         <v>231</v>
       </c>
@@ -3427,7 +3514,7 @@
       <c r="J79" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="M79" s="14" t="s">
+      <c r="M79" s="32" t="s">
         <v>70</v>
       </c>
       <c r="N79" s="14" t="s">
@@ -3447,7 +3534,7 @@
       <c r="H80" t="s">
         <v>51</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M80" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N80" t="s">
@@ -3467,7 +3554,7 @@
       <c r="H81" t="s">
         <v>55</v>
       </c>
-      <c r="M81" t="s">
+      <c r="M81" s="31" t="s">
         <v>56</v>
       </c>
       <c r="N81" t="s">
@@ -3487,7 +3574,7 @@
       <c r="H82" t="s">
         <v>235</v>
       </c>
-      <c r="M82" t="s">
+      <c r="M82" s="31" t="s">
         <v>22</v>
       </c>
       <c r="N82" t="s">
@@ -3501,13 +3588,14 @@
       <c r="A83" s="13" t="s">
         <v>233</v>
       </c>
+      <c r="D83" s="22"/>
       <c r="E83" s="14" t="s">
         <v>234</v>
       </c>
       <c r="H83" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="M83" s="14" t="s">
+      <c r="M83" s="32" t="s">
         <v>22</v>
       </c>
       <c r="N83" s="14" t="s">
@@ -3521,13 +3609,14 @@
       <c r="A84" s="13" t="s">
         <v>236</v>
       </c>
+      <c r="D84" s="22"/>
       <c r="E84" s="14" t="s">
         <v>237</v>
       </c>
       <c r="H84" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="M84" s="14" t="s">
+      <c r="M84" s="32" t="s">
         <v>15</v>
       </c>
       <c r="N84" s="14" t="s">
@@ -3547,7 +3636,7 @@
       <c r="H85" t="s">
         <v>238</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M85" s="31" t="s">
         <v>21</v>
       </c>
       <c r="N85" t="s">
@@ -3567,7 +3656,7 @@
       <c r="H86" t="s">
         <v>238</v>
       </c>
-      <c r="M86" t="s">
+      <c r="M86" s="31" t="s">
         <v>25</v>
       </c>
       <c r="N86" t="s">
@@ -3587,7 +3676,7 @@
       <c r="H87" t="s">
         <v>242</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M87" s="31" t="s">
         <v>81</v>
       </c>
       <c r="N87" t="s">
@@ -3607,7 +3696,7 @@
       <c r="H88" t="s">
         <v>242</v>
       </c>
-      <c r="M88" t="s">
+      <c r="M88" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N88" t="s">
@@ -3627,7 +3716,7 @@
       <c r="H89" t="s">
         <v>248</v>
       </c>
-      <c r="M89" t="s">
+      <c r="M89" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N89" t="s">
@@ -3653,7 +3742,7 @@
       <c r="I90" t="s">
         <v>252</v>
       </c>
-      <c r="M90" t="s">
+      <c r="M90" s="31" t="s">
         <v>81</v>
       </c>
       <c r="N90" t="s">
@@ -3673,7 +3762,7 @@
       <c r="H91" t="s">
         <v>107</v>
       </c>
-      <c r="M91" t="s">
+      <c r="M91" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N91" t="s">
@@ -3693,7 +3782,7 @@
       <c r="H92" t="s">
         <v>107</v>
       </c>
-      <c r="M92" t="s">
+      <c r="M92" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N92" t="s">
@@ -3713,7 +3802,7 @@
       <c r="H93" t="s">
         <v>107</v>
       </c>
-      <c r="M93" t="s">
+      <c r="M93" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N93" t="s">
@@ -3733,7 +3822,7 @@
       <c r="H94" t="s">
         <v>107</v>
       </c>
-      <c r="M94" t="s">
+      <c r="M94" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N94" t="s">
@@ -3753,7 +3842,7 @@
       <c r="H95" t="s">
         <v>107</v>
       </c>
-      <c r="M95" t="s">
+      <c r="M95" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N95" t="s">
@@ -3773,7 +3862,7 @@
       <c r="H96" t="s">
         <v>252</v>
       </c>
-      <c r="M96" t="s">
+      <c r="M96" s="31" t="s">
         <v>81</v>
       </c>
       <c r="N96" t="s">
@@ -3793,7 +3882,7 @@
       <c r="H97" t="s">
         <v>18</v>
       </c>
-      <c r="M97" t="s">
+      <c r="M97" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N97" t="s">
@@ -3813,7 +3902,7 @@
       <c r="H98" t="s">
         <v>258</v>
       </c>
-      <c r="M98" t="s">
+      <c r="M98" s="31" t="s">
         <v>15</v>
       </c>
       <c r="N98" t="s">
@@ -3833,7 +3922,7 @@
       <c r="H99" t="s">
         <v>259</v>
       </c>
-      <c r="M99" t="s">
+      <c r="M99" s="31" t="s">
         <v>81</v>
       </c>
       <c r="N99" t="s">
@@ -3853,7 +3942,7 @@
       <c r="H100" t="s">
         <v>110</v>
       </c>
-      <c r="M100" t="s">
+      <c r="M100" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N100" t="s">
@@ -3873,7 +3962,7 @@
       <c r="H101" t="s">
         <v>110</v>
       </c>
-      <c r="M101" t="s">
+      <c r="M101" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N101" t="s">
@@ -3894,7 +3983,7 @@
       <c r="H102" t="s">
         <v>110</v>
       </c>
-      <c r="M102" t="s">
+      <c r="M102" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N102" t="s">
@@ -3914,7 +4003,7 @@
       <c r="H103" t="s">
         <v>110</v>
       </c>
-      <c r="M103" t="s">
+      <c r="M103" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N103" t="s">
@@ -3934,7 +4023,7 @@
       <c r="H104" t="s">
         <v>64</v>
       </c>
-      <c r="M104" t="s">
+      <c r="M104" s="31" t="s">
         <v>65</v>
       </c>
       <c r="N104" t="s">
@@ -3950,7 +4039,7 @@
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
+      <c r="D105" s="25"/>
       <c r="E105" s="4" t="s">
         <v>133</v>
       </c>
@@ -3963,7 +4052,7 @@
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="4" t="s">
+      <c r="M105" s="35" t="s">
         <v>135</v>
       </c>
       <c r="N105" s="4" t="s">
@@ -3983,7 +4072,7 @@
       <c r="H106" t="s">
         <v>134</v>
       </c>
-      <c r="M106" t="s">
+      <c r="M106" s="31" t="s">
         <v>15</v>
       </c>
       <c r="N106" t="s">
@@ -4003,7 +4092,7 @@
       <c r="H107" t="s">
         <v>134</v>
       </c>
-      <c r="M107" t="s">
+      <c r="M107" s="31" t="s">
         <v>135</v>
       </c>
       <c r="N107" t="s">
@@ -4023,7 +4112,7 @@
       <c r="H108" t="s">
         <v>134</v>
       </c>
-      <c r="M108" t="s">
+      <c r="M108" s="31" t="s">
         <v>15</v>
       </c>
       <c r="N108" t="s">
@@ -4037,13 +4126,14 @@
       <c r="A109" s="13" t="s">
         <v>260</v>
       </c>
+      <c r="D109" s="22"/>
       <c r="E109" s="14" t="s">
         <v>256</v>
       </c>
       <c r="H109" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="M109" s="14" t="s">
+      <c r="M109" s="32" t="s">
         <v>153</v>
       </c>
       <c r="N109" s="14" t="s">
@@ -4063,7 +4153,7 @@
       <c r="H110" t="s">
         <v>265</v>
       </c>
-      <c r="M110" t="s">
+      <c r="M110" s="31" t="s">
         <v>31</v>
       </c>
       <c r="N110" t="s">
@@ -4079,7 +4169,7 @@
       </c>
       <c r="B111" s="14"/>
       <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
+      <c r="D111" s="22"/>
       <c r="E111" s="14" t="s">
         <v>68</v>
       </c>
@@ -4092,7 +4182,7 @@
       <c r="J111" s="14"/>
       <c r="K111" s="14"/>
       <c r="L111" s="14"/>
-      <c r="M111" s="14" t="s">
+      <c r="M111" s="32" t="s">
         <v>77</v>
       </c>
       <c r="N111" s="14" t="s">
@@ -4108,7 +4198,7 @@
       </c>
       <c r="B112"/>
       <c r="C112"/>
-      <c r="D112"/>
+      <c r="D112" s="21"/>
       <c r="E112" t="s">
         <v>79</v>
       </c>
@@ -4121,7 +4211,7 @@
       <c r="J112"/>
       <c r="K112"/>
       <c r="L112"/>
-      <c r="M112" t="s">
+      <c r="M112" s="31" t="s">
         <v>81</v>
       </c>
       <c r="N112" t="s">
@@ -4147,7 +4237,7 @@
       <c r="I113" t="s">
         <v>86</v>
       </c>
-      <c r="M113" t="s">
+      <c r="M113" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N113" t="s">
@@ -4161,13 +4251,14 @@
       <c r="A114" s="13" t="s">
         <v>269</v>
       </c>
+      <c r="D114" s="22"/>
       <c r="E114" s="14" t="s">
         <v>270</v>
       </c>
       <c r="H114" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="M114" s="14" t="s">
+      <c r="M114" s="32" t="s">
         <v>52</v>
       </c>
       <c r="N114" s="14" t="s">
@@ -4187,7 +4278,7 @@
       <c r="H115" t="s">
         <v>273</v>
       </c>
-      <c r="M115" t="s">
+      <c r="M115" s="31" t="s">
         <v>56</v>
       </c>
       <c r="N115" t="s">
@@ -4203,7 +4294,7 @@
       </c>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
+      <c r="D116" s="29"/>
       <c r="E116" s="6" t="s">
         <v>188</v>
       </c>
@@ -4216,7 +4307,7 @@
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
-      <c r="M116" s="6" t="s">
+      <c r="M116" s="39" t="s">
         <v>159</v>
       </c>
       <c r="N116" s="6" t="s">
@@ -4236,7 +4327,7 @@
       <c r="H117" t="s">
         <v>189</v>
       </c>
-      <c r="M117" t="s">
+      <c r="M117" s="31" t="s">
         <v>159</v>
       </c>
       <c r="N117" t="s">
@@ -4250,13 +4341,14 @@
       <c r="A118" s="13" t="s">
         <v>187</v>
       </c>
+      <c r="D118" s="22"/>
       <c r="E118" s="14" t="s">
         <v>188</v>
       </c>
       <c r="H118" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="M118" s="14" t="s">
+      <c r="M118" s="32" t="s">
         <v>159</v>
       </c>
       <c r="N118" s="14" t="s">
@@ -4270,13 +4362,14 @@
       <c r="A119" s="13" t="s">
         <v>261</v>
       </c>
+      <c r="D119" s="22"/>
       <c r="E119" s="14" t="s">
         <v>262</v>
       </c>
       <c r="H119" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="M119" s="14" t="s">
+      <c r="M119" s="32" t="s">
         <v>56</v>
       </c>
       <c r="N119" s="14" t="s">
@@ -4296,7 +4389,7 @@
       <c r="H120" t="s">
         <v>263</v>
       </c>
-      <c r="M120" t="s">
+      <c r="M120" s="31" t="s">
         <v>56</v>
       </c>
       <c r="N120" t="s">
@@ -4310,13 +4403,14 @@
       <c r="A121" s="13" t="s">
         <v>274</v>
       </c>
+      <c r="D121" s="22"/>
       <c r="E121" s="14" t="s">
         <v>275</v>
       </c>
       <c r="H121" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="M121" s="14" t="s">
+      <c r="M121" s="32" t="s">
         <v>60</v>
       </c>
       <c r="N121" s="14" t="s">
@@ -4330,13 +4424,14 @@
       <c r="A122" s="13" t="s">
         <v>279</v>
       </c>
+      <c r="D122" s="22"/>
       <c r="E122" s="14" t="s">
         <v>280</v>
       </c>
       <c r="H122" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="M122" s="14" t="s">
+      <c r="M122" s="32" t="s">
         <v>60</v>
       </c>
       <c r="N122" s="14" t="s">
@@ -4356,7 +4451,7 @@
       <c r="H123" t="s">
         <v>284</v>
       </c>
-      <c r="M123" t="s">
+      <c r="M123" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N123" t="s">
@@ -4376,7 +4471,7 @@
       <c r="H124" t="s">
         <v>287</v>
       </c>
-      <c r="M124" t="s">
+      <c r="M124" s="31" t="s">
         <v>52</v>
       </c>
       <c r="N124" t="s">
@@ -4396,7 +4491,7 @@
       <c r="H125" t="s">
         <v>294</v>
       </c>
-      <c r="M125" t="s">
+      <c r="M125" s="31" t="s">
         <v>47</v>
       </c>
       <c r="N125" t="s">
@@ -4412,7 +4507,7 @@
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
+      <c r="D126" s="25"/>
       <c r="E126" s="4" t="s">
         <v>296</v>
       </c>
@@ -4425,7 +4520,7 @@
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
       <c r="L126" s="4"/>
-      <c r="M126" s="4" t="s">
+      <c r="M126" s="35" t="s">
         <v>56</v>
       </c>
       <c r="N126" s="4" t="s">
@@ -4445,7 +4540,7 @@
       <c r="H127" t="s">
         <v>300</v>
       </c>
-      <c r="M127" t="s">
+      <c r="M127" s="31" t="s">
         <v>60</v>
       </c>
       <c r="N127" t="s">

</xml_diff>